<commit_message>
Update end time - Sabrina timesheet
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/Contributions/TimeReport_SabrinaLuu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB90A81-CEE3-4FFF-AC8E-C8063BF414F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9831CF6-E364-40D6-B162-8608056E5A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Name:</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Reformatting and refactoring homeView, post.dart, and remote_service</t>
+  </si>
+  <si>
+    <t>Display plant data on the home screen and add refresh button to manually pull information from backend</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -731,7 +734,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E201)</f>
-        <v>1.1381944444444447</v>
+        <v>1.9041666666666672</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -1125,12 +1128,16 @@
       <c r="C21" s="9">
         <v>0.61736111111111114</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="9">
+        <v>0.76597222222222228</v>
+      </c>
       <c r="E21" s="10">
         <f t="shared" si="0"/>
-        <v>-0.61736111111111114</v>
-      </c>
-      <c r="F21" s="15"/>
+        <v>0.14861111111111114</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>

</xml_diff>

<commit_message>
Temp placeholder update for now
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/Contributions/TimeReport_SabrinaLuu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\TimeSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB90A81-CEE3-4FFF-AC8E-C8063BF414F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D340B5-BA9E-43C0-B989-538DAC0CBEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Name:</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Reformatting and refactoring homeView, post.dart, and remote_service</t>
+  </si>
+  <si>
+    <t>Formatted parsed JSON data pulled from the backend and created a plant card widget to display on the home screen.</t>
+  </si>
+  <si>
+    <t>Testing new plant card format with the backend, implemented refresh button under plant info card, making sure it properly GETs updated data from backend server</t>
+  </si>
+  <si>
+    <t>Helped Nick attempt to test new IP for mobile app to pull from backend server, need to run frontend and backend locally</t>
+  </si>
+  <si>
+    <t>Prototype Dev</t>
+  </si>
+  <si>
+    <t>Found commands to run the mobile app from the terminal, ease of compiling. Collected data for report and formatted mobile app architecture for efficiency</t>
+  </si>
+  <si>
+    <t>Working on presentation, listing Design 2 milestones based on Design 1 completed work and timeline for future goals</t>
   </si>
 </sst>
 </file>
@@ -323,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -362,6 +380,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,8 +754,8 @@
         <v>10</v>
       </c>
       <c r="E1" s="6">
-        <f>SUM(E4:E201)</f>
-        <v>1.1381944444444447</v>
+        <f>SUM(E4:E202)</f>
+        <v>2.4486111111111115</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -812,7 +836,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" ref="E6:E70" si="0">D6-C6</f>
+        <f t="shared" ref="E6:E71" si="0">D6-C6</f>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -1096,23 +1120,23 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="9">
-        <v>0.57986111111111116</v>
+        <v>0.8</v>
       </c>
       <c r="D20" s="9">
-        <v>0.60277777777777775</v>
+        <v>0.9770833333333333</v>
       </c>
       <c r="E20" s="10">
         <f t="shared" si="0"/>
-        <v>2.2916666666666585E-2</v>
+        <v>0.17708333333333326</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1123,58 +1147,102 @@
         <v>23</v>
       </c>
       <c r="C21" s="9">
+        <v>0.57986111111111116</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>2.2916666666666585E-2</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>45975</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="9">
         <v>0.61736111111111114</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="10">
-        <f t="shared" si="0"/>
-        <v>-0.61736111111111114</v>
-      </c>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="D22" s="9">
+        <v>0.76597222222222228</v>
+      </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="15"/>
+        <v>0.14861111111111114</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="A23" s="18">
+        <v>45976</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.62777777777777777</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.7055555555555556</v>
+      </c>
       <c r="E23" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="15"/>
+        <v>7.7777777777777835E-2</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="7">
+        <v>45977</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.55138888888888893</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.7270833333333333</v>
+      </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="15"/>
+        <v>0.17569444444444438</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="7">
+        <v>45978</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="19">
+        <v>0.7680555555555556</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.88194444444444442</v>
+      </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="15"/>
+        <v>0.11388888888888882</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
@@ -1677,7 +1745,7 @@
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="10">
-        <f t="shared" ref="E71:E134" si="1">D71-C71</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F71" s="15"/>
@@ -1688,7 +1756,7 @@
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E72:E135" si="1">D72-C72</f>
         <v>0</v>
       </c>
       <c r="F72" s="15"/>
@@ -2381,7 +2449,7 @@
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
       <c r="E135" s="10">
-        <f t="shared" ref="E135:E198" si="2">D135-C135</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F135" s="15"/>
@@ -2392,7 +2460,7 @@
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E136:E199" si="2">D136-C136</f>
         <v>0</v>
       </c>
       <c r="F136" s="15"/>
@@ -3085,7 +3153,7 @@
       <c r="C199" s="8"/>
       <c r="D199" s="8"/>
       <c r="E199" s="10">
-        <f t="shared" ref="E199:E201" si="3">D199-C199</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F199" s="15"/>
@@ -3096,21 +3164,32 @@
       <c r="C200" s="8"/>
       <c r="D200" s="8"/>
       <c r="E200" s="10">
+        <f t="shared" ref="E200:E202" si="3">D200-C200</f>
+        <v>0</v>
+      </c>
+      <c r="F200" s="15"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="11"/>
+      <c r="B201" s="8"/>
+      <c r="C201" s="8"/>
+      <c r="D201" s="8"/>
+      <c r="E201" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F200" s="15"/>
-    </row>
-    <row r="201" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="12"/>
-      <c r="B201" s="13"/>
-      <c r="C201" s="13"/>
-      <c r="D201" s="13"/>
-      <c r="E201" s="14">
+      <c r="F201" s="15"/>
+    </row>
+    <row r="202" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="12"/>
+      <c r="B202" s="13"/>
+      <c r="C202" s="13"/>
+      <c r="D202" s="13"/>
+      <c r="E202" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F201" s="16"/>
+      <c r="F202" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>